<commit_message>
add newest result on whole gene data
git-svn-id: svn://svn.r-forge.r-project.org/svnroot/proteinevoutk20@300 edb9625f-4e0d-4859-8d74-9fd3b1da38cb
</commit_message>
<xml_diff>
--- a/pkg/Result/loglik_comp.xlsx
+++ b/pkg/Result/loglik_comp.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="945" yWindow="915" windowWidth="28440" windowHeight="13980"/>
+    <workbookView xWindow="315" yWindow="-105" windowWidth="28440" windowHeight="13980" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="WholeSeq" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
   <si>
     <t>maxll</t>
   </si>
@@ -43,15 +44,46 @@
   <si>
     <t>loglik_opw_all</t>
   </si>
+  <si>
+    <t>edge length</t>
+  </si>
+  <si>
+    <t>Max</t>
+  </si>
+  <si>
+    <t>sensitivity</t>
+  </si>
+  <si>
+    <t>mutation rates</t>
+  </si>
+  <si>
+    <t>Grantham weights</t>
+  </si>
+  <si>
+    <t>Maj</t>
+  </si>
+  <si>
+    <t>Opw</t>
+  </si>
+  <si>
+    <t>opw</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,8 +109,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -375,7 +408,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D107"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1893,11 +1926,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E107"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="17.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="3" max="3" width="16.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -3721,4 +3761,389 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:U16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1">
+        <v>-239736.4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>8.9072029999999996E-2</v>
+      </c>
+      <c r="C2">
+        <v>0.11949037999999999</v>
+      </c>
+      <c r="D2">
+        <v>7.2600570000000003E-2</v>
+      </c>
+      <c r="E2">
+        <v>0.19425756999999999</v>
+      </c>
+      <c r="F2">
+        <v>0.25679729000000001</v>
+      </c>
+      <c r="G2">
+        <v>7.5944170000000005E-2</v>
+      </c>
+      <c r="H2">
+        <v>7.1705089999999999E-2</v>
+      </c>
+      <c r="I2">
+        <v>0.27035913</v>
+      </c>
+      <c r="J2">
+        <v>1.8938912800000001</v>
+      </c>
+      <c r="K2">
+        <v>1.4601866800000001</v>
+      </c>
+      <c r="L2">
+        <v>0.7815145</v>
+      </c>
+      <c r="M2">
+        <v>1.5326933</v>
+      </c>
+      <c r="N2">
+        <v>1.62200615</v>
+      </c>
+      <c r="O2">
+        <v>3.31342508</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21">
+      <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1.7699400000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>7.9876440000000004</v>
+      </c>
+      <c r="C4">
+        <v>17.861460999999998</v>
+      </c>
+      <c r="D4">
+        <v>5.494853</v>
+      </c>
+      <c r="E4">
+        <v>5.4875410000000002</v>
+      </c>
+      <c r="F4">
+        <v>18.971951000000001</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>1.829271654</v>
+      </c>
+      <c r="C5">
+        <v>0.115927294</v>
+      </c>
+      <c r="D5">
+        <v>5.6583200000000005E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1">
+        <v>-257790.1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0.20092260000000001</v>
+      </c>
+      <c r="C7">
+        <v>0.2810494</v>
+      </c>
+      <c r="D7">
+        <v>0.28218409999999999</v>
+      </c>
+      <c r="E7">
+        <v>0.3710658</v>
+      </c>
+      <c r="F7">
+        <v>0.46659859999999997</v>
+      </c>
+      <c r="G7">
+        <v>0.29916019999999999</v>
+      </c>
+      <c r="H7">
+        <v>0.3943893</v>
+      </c>
+      <c r="I7">
+        <v>0.26162150000000001</v>
+      </c>
+      <c r="J7">
+        <v>0.35944520000000002</v>
+      </c>
+      <c r="K7">
+        <v>3.6674981</v>
+      </c>
+      <c r="L7">
+        <v>0.75001430000000002</v>
+      </c>
+      <c r="M7">
+        <v>0.71580010000000005</v>
+      </c>
+      <c r="N7">
+        <v>0.98276240000000004</v>
+      </c>
+      <c r="O7">
+        <v>1.3953857999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>1.522956</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>6.1003970000000001</v>
+      </c>
+      <c r="C9">
+        <v>12.804228</v>
+      </c>
+      <c r="D9">
+        <v>3.815404</v>
+      </c>
+      <c r="E9">
+        <v>4.237978</v>
+      </c>
+      <c r="F9">
+        <v>9.0234159999999992</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>1.8292716544000001</v>
+      </c>
+      <c r="C10">
+        <v>0.18168360089999999</v>
+      </c>
+      <c r="D10">
+        <v>6.9448839999999997E-4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="1">
+        <v>-319625.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>2.859037E-2</v>
+      </c>
+      <c r="C12">
+        <v>3.747785E-2</v>
+      </c>
+      <c r="D12">
+        <v>2.2736579999999999E-2</v>
+      </c>
+      <c r="E12">
+        <v>5.9882770000000002E-2</v>
+      </c>
+      <c r="F12">
+        <v>8.1207440000000006E-2</v>
+      </c>
+      <c r="G12">
+        <v>1.9532629999999999E-2</v>
+      </c>
+      <c r="H12">
+        <v>2.9443029999999999E-2</v>
+      </c>
+      <c r="I12">
+        <v>7.6313790000000006E-2</v>
+      </c>
+      <c r="J12">
+        <v>0.39991033999999998</v>
+      </c>
+      <c r="K12">
+        <v>0.29173226000000002</v>
+      </c>
+      <c r="L12">
+        <v>0.14150011000000001</v>
+      </c>
+      <c r="M12">
+        <v>0.37782304999999999</v>
+      </c>
+      <c r="N12">
+        <v>0.67028500999999996</v>
+      </c>
+      <c r="O12">
+        <v>0.50702464000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1.613693</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>2.3447990000000001</v>
+      </c>
+      <c r="C14">
+        <v>4.6895740000000004</v>
+      </c>
+      <c r="D14">
+        <v>1.4925679999999999</v>
+      </c>
+      <c r="E14">
+        <v>1.5559069999999999</v>
+      </c>
+      <c r="F14">
+        <v>1.623264</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>1.8292716544000001</v>
+      </c>
+      <c r="C15">
+        <v>0.10400940960000001</v>
+      </c>
+      <c r="D15">
+        <v>3.2731930000000001E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21">
+      <c r="A16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16">
+        <v>0.103060992</v>
+      </c>
+      <c r="C16">
+        <v>0.12839119299999999</v>
+      </c>
+      <c r="D16">
+        <v>8.4753555999999994E-2</v>
+      </c>
+      <c r="E16">
+        <v>5.8870736999999999E-2</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>3.4413239999999999E-3</v>
+      </c>
+      <c r="H16">
+        <v>7.0437266999999998E-2</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>3.4521514000000003E-2</v>
+      </c>
+      <c r="L16">
+        <v>0.14672855300000001</v>
+      </c>
+      <c r="M16">
+        <v>7.0399829999999997E-3</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0.14560948400000001</v>
+      </c>
+      <c r="R16">
+        <v>0</v>
+      </c>
+      <c r="S16">
+        <v>0</v>
+      </c>
+      <c r="T16">
+        <v>0.21714539699999999</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>